<commit_message>
Added way to retrieve newly started recording
</commit_message>
<xml_diff>
--- a/extras/sample-form/Sample form - Delete Twilio recording.xlsx
+++ b/extras/sample-form/Sample form - Delete Twilio recording.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Dobility support/Field plug-ins/Plug-ins by Max/In progress/twilio-control/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43BF6124-7E9A-3C4F-BC48-C3C710180AE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76ADF35C-3A2E-F842-8E4C-705F1745B768}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="460" windowWidth="28800" windowHeight="16720" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="480" windowWidth="28800" windowHeight="16720" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="429">
   <si>
     <t>type</t>
   </si>
@@ -2739,9 +2739,6 @@
   </si>
   <si>
     <t>custom-twilio-call(from_number=${your_number},to_number=${number_to_call},twilio_number=${twilio_number},account_sid=${twilio_sid},auth_token=${twilio_auth},record=${record_call},display_number=${display_number})</t>
-  </si>
-  <si>
-    <t>If consent is withheld, the recording will be deleted</t>
   </si>
   <si>
     <t>Delete Twilio recording</t>
@@ -2771,6 +2768,12 @@
   </si>
   <si>
     <t>custom-twilio-control(action=${action}, call_url=${twilio_call_url}, auth_token=${twilio_auth})</t>
+  </si>
+  <si>
+    <t>new_twilio_call_recordings_url</t>
+  </si>
+  <si>
+    <t>item-at('|', plug-in-metadata(${recording_consent}), 1)</t>
   </si>
 </sst>
 </file>
@@ -3230,7 +3233,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3392,6 +3395,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="108">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -4944,11 +4948,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W29"/>
+  <dimension ref="A1:W30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5220,7 +5224,7 @@
         <v>410</v>
       </c>
       <c r="C12" s="55" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D12" s="56"/>
       <c r="E12" s="54"/>
@@ -5516,13 +5520,13 @@
     </row>
     <row r="26" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>420</v>
+      </c>
+      <c r="B26" s="58" t="s">
         <v>421</v>
       </c>
-      <c r="B26" s="58" t="s">
+      <c r="C26" s="55" t="s">
         <v>422</v>
-      </c>
-      <c r="C26" s="55" t="s">
-        <v>423</v>
       </c>
       <c r="F26" s="56"/>
       <c r="K26" s="54"/>
@@ -5539,11 +5543,8 @@
       <c r="C27" s="21" t="s">
         <v>415</v>
       </c>
-      <c r="D27" s="11" t="s">
-        <v>418</v>
-      </c>
       <c r="F27" s="21" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="K27" t="s">
         <v>379</v>
@@ -5553,26 +5554,41 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>139</v>
+      </c>
+      <c r="B28" s="58" t="s">
+        <v>427</v>
+      </c>
+      <c r="C28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="K28"/>
+      <c r="N28" s="71" t="s">
+        <v>428</v>
+      </c>
+      <c r="O28"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>155</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="68" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="30" spans="1:15" ht="68" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>33</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>398</v>
       </c>
-      <c r="C29" s="21" t="s">
+      <c r="C30" s="21" t="s">
         <v>399</v>
       </c>
-      <c r="I29" t="s">
+      <c r="I30" t="s">
         <v>400</v>
       </c>
-      <c r="K29" t="s">
+      <c r="K30" t="s">
         <v>374</v>
       </c>
     </row>
@@ -5726,7 +5742,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5779,29 +5795,29 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>24</v>
@@ -5855,7 +5871,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5890,14 +5908,14 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
+        <v>418</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>419</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>420</v>
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2008282033</v>
+        <v>2008282106</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>359</v>

</xml_diff>

<commit_message>
Updated sample form with more customization
</commit_message>
<xml_diff>
--- a/extras/sample-form/Sample form - Delete Twilio recording.xlsx
+++ b/extras/sample-form/Sample form - Delete Twilio recording.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Dobility support/Field plug-ins/Plug-ins by Max/In progress/twilio-control/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76ADF35C-3A2E-F842-8E4C-705F1745B768}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4804BD-F1F3-0647-A499-A6F66FAD54D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="480" windowWidth="28800" windowHeight="16720" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28780" yWindow="460" windowWidth="28800" windowHeight="16720" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="436">
   <si>
     <t>type</t>
   </si>
@@ -2762,18 +2762,39 @@
     <t>stop</t>
   </si>
   <si>
-    <t>&lt;p&gt;Welcome to this SurveyCTO sample form on the twilio-control field plug-in!&lt;/p&gt;
+    <t>custom-twilio-control(action=${action}, call_url=${twilio_call_url}, auth_token=${twilio_auth})</t>
+  </si>
+  <si>
+    <t>new_twilio_call_recordings_url</t>
+  </si>
+  <si>
+    <t>plug-in-metadata(${recording_consent})</t>
+  </si>
+  <si>
+    <t>recording_metadata</t>
+  </si>
+  <si>
+    <t>recording_success_code</t>
+  </si>
+  <si>
+    <t>item-at('|', ${recording_metadata}, 1)</t>
+  </si>
+  <si>
+    <t>item-at('|', ${recording_metadata}, 0)</t>
+  </si>
+  <si>
+    <t>Metadata</t>
+  </si>
+  <si>
+    <t>Success code: 0, 1, or 2</t>
+  </si>
+  <si>
+    <t>Either a message about the success, or a URL to the new recording.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welcome to this SurveyCTO sample form for the twilio-control field plug-in!&lt;/p&gt;
 &lt;br&gt;
 &lt;p&gt;Here, a call recording can be stopped, started, or even deleted. Check out the &lt;a href="https://github.com/SurveyCTO/twilio-control/tree/master/README.md" target="_blank"&gt;readme&lt;/a&gt; to learn more.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>custom-twilio-control(action=${action}, call_url=${twilio_call_url}, auth_token=${twilio_auth})</t>
-  </si>
-  <si>
-    <t>new_twilio_call_recordings_url</t>
-  </si>
-  <si>
-    <t>item-at('|', plug-in-metadata(${recording_consent}), 1)</t>
   </si>
 </sst>
 </file>
@@ -3233,7 +3254,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3396,6 +3417,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="108">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -4948,11 +4970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W30"/>
+  <dimension ref="A1:W32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5224,7 +5248,7 @@
         <v>410</v>
       </c>
       <c r="C12" s="55" t="s">
-        <v>425</v>
+        <v>435</v>
       </c>
       <c r="D12" s="56"/>
       <c r="E12" s="54"/>
@@ -5383,8 +5407,8 @@
       <c r="C18" s="21" t="s">
         <v>385</v>
       </c>
-      <c r="E18" t="s">
-        <v>361</v>
+      <c r="E18" s="72">
+        <v>1</v>
       </c>
       <c r="K18" t="s">
         <v>379</v>
@@ -5527,6 +5551,9 @@
       </c>
       <c r="C26" s="55" t="s">
         <v>422</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>423</v>
       </c>
       <c r="F26" s="56"/>
       <c r="K26" s="54"/>
@@ -5544,7 +5571,7 @@
         <v>415</v>
       </c>
       <c r="F27" s="21" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="K27" t="s">
         <v>379</v>
@@ -5552,43 +5579,79 @@
       <c r="N27" s="54"/>
       <c r="O27"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>139</v>
       </c>
       <c r="B28" s="58" t="s">
-        <v>427</v>
-      </c>
-      <c r="C28" s="21"/>
+        <v>428</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>432</v>
+      </c>
       <c r="F28" s="21"/>
       <c r="K28"/>
       <c r="N28" s="71" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="O28"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>139</v>
+      </c>
+      <c r="B29" s="58" t="s">
+        <v>429</v>
+      </c>
+      <c r="C29" s="21" t="s">
+        <v>433</v>
+      </c>
+      <c r="F29" s="21"/>
+      <c r="K29"/>
+      <c r="N29" s="71" t="s">
+        <v>431</v>
+      </c>
+      <c r="O29"/>
+    </row>
+    <row r="30" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>139</v>
+      </c>
+      <c r="B30" s="58" t="s">
+        <v>426</v>
+      </c>
+      <c r="C30" s="21" t="s">
+        <v>434</v>
+      </c>
+      <c r="F30" s="21"/>
+      <c r="K30"/>
+      <c r="N30" s="71" t="s">
+        <v>430</v>
+      </c>
+      <c r="O30"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>155</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B31" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="68" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="32" spans="1:15" ht="68" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>33</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B32" t="s">
         <v>398</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="C32" s="21" t="s">
         <v>399</v>
       </c>
-      <c r="I30" t="s">
+      <c r="I32" t="s">
         <v>400</v>
       </c>
-      <c r="K30" t="s">
+      <c r="K32" t="s">
         <v>374</v>
       </c>
     </row>
@@ -5915,7 +5978,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2008282106</v>
+        <v>2008291916</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>359</v>

</xml_diff>

<commit_message>
Removed metadata check from repeat group
</commit_message>
<xml_diff>
--- a/extras/sample-form/Sample form - Delete Twilio recording.xlsx
+++ b/extras/sample-form/Sample form - Delete Twilio recording.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Dobility support/Field plug-ins/Plug-ins by Max/In progress/twilio-control/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4804BD-F1F3-0647-A499-A6F66FAD54D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E6ADAD-BAF2-134E-B0F4-57DE7C63B0A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28780" yWindow="460" windowWidth="28800" windowHeight="16720" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28740" yWindow="460" windowWidth="28800" windowHeight="16720" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="448">
   <si>
     <t>type</t>
   </si>
@@ -2672,9 +2672,6 @@
     <t>pulldata('twilio_access', 'number', 'accessid_key', 1234)</t>
   </si>
   <si>
-    <t>call_attempt</t>
-  </si>
-  <si>
     <t>Call attempt</t>
   </si>
   <si>
@@ -2732,9 +2729,6 @@
     <t>recording_consent</t>
   </si>
   <si>
-    <t>Does the respondent give consent for the call to be recorded?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Twilio SID number for the call. Field plug-in metadata position 1. </t>
   </si>
   <si>
@@ -2753,16 +2747,10 @@
     <t>action</t>
   </si>
   <si>
-    <t>Which action should be taken?</t>
-  </si>
-  <si>
     <t>delete</t>
   </si>
   <si>
     <t>stop</t>
-  </si>
-  <si>
-    <t>custom-twilio-control(action=${action}, call_url=${twilio_call_url}, auth_token=${twilio_auth})</t>
   </si>
   <si>
     <t>new_twilio_call_recordings_url</t>
@@ -2795,6 +2783,55 @@
     <t>&lt;p&gt;Welcome to this SurveyCTO sample form for the twilio-control field plug-in!&lt;/p&gt;
 &lt;br&gt;
 &lt;p&gt;Here, a call recording can be stopped, started, or even deleted. Check out the &lt;a href="https://github.com/SurveyCTO/twilio-control/tree/master/README.md" target="_blank"&gt;readme&lt;/a&gt; to learn more.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>answered</t>
+  </si>
+  <si>
+    <t>Did someone answer the phone (either the respondent or anyone else)?</t>
+  </si>
+  <si>
+    <t>no_answer</t>
+  </si>
+  <si>
+    <t>ENUMERATOR: If you get the opportunity to leave a voicemail, leave the following:
+Hi [respondent's name], this is [your name] regarding a survey. Can you please call us back when you get a chance at XXX-XXX-XXXX? Again, that's XXX-XXX-XXXX. Thanks!</t>
+  </si>
+  <si>
+    <t>Hi [respondent's name], this is [your name] regarding a survey. Is it okay if we record this call?</t>
+  </si>
+  <si>
+    <t>selected(${answered}, '0')</t>
+  </si>
+  <si>
+    <t>num_calls</t>
+  </si>
+  <si>
+    <t>${num_calls}</t>
+  </si>
+  <si>
+    <t>Which action should be taken in this example?</t>
+  </si>
+  <si>
+    <t>last_call_url</t>
+  </si>
+  <si>
+    <t>custom-twilio-control(action=${action}, call_url=${last_call_url}, auth_token=${twilio_auth})</t>
+  </si>
+  <si>
+    <t>indexed-repeat(${twilio_call_url}, ${call_attempts}, count(${answered}))</t>
+  </si>
+  <si>
+    <t>another_call</t>
+  </si>
+  <si>
+    <t>Is there another phone number you can call?</t>
+  </si>
+  <si>
+    <t>sum(${answered}) &gt; 0</t>
+  </si>
+  <si>
+    <t>sum(${another_call}) + 1</t>
   </si>
 </sst>
 </file>
@@ -3382,6 +3419,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3415,9 +3455,6 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="108">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -4970,13 +5007,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W32"/>
+  <dimension ref="A1:W39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomRight" activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5228,8 +5265,8 @@
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A11" s="70"/>
-      <c r="B11" s="70"/>
+      <c r="A11" s="59"/>
+      <c r="B11" s="59"/>
       <c r="C11" s="55"/>
       <c r="D11" s="56"/>
       <c r="E11" s="54"/>
@@ -5245,15 +5282,15 @@
         <v>33</v>
       </c>
       <c r="B12" s="57" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C12" s="55" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="D12" s="56"/>
       <c r="E12" s="54"/>
       <c r="F12" s="56" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
@@ -5265,47 +5302,38 @@
     </row>
     <row r="13" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>418</v>
+      </c>
+      <c r="B13" s="58" t="s">
+        <v>419</v>
+      </c>
+      <c r="C13" s="55" t="s">
+        <v>440</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>420</v>
+      </c>
+      <c r="F13" s="56"/>
+      <c r="K13" s="54"/>
+      <c r="N13"/>
+      <c r="O13" s="54"/>
+    </row>
+    <row r="14" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>139</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>389</v>
       </c>
-      <c r="C13" s="53" t="str">
+      <c r="C14" s="53" t="str">
         <f>HYPERLINK("https://www.twilio.com/docs/glossary/what-is-a-sid","Twilio String Identifier (SID)")</f>
         <v>Twilio String Identifier (SID)</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D14" s="21" t="s">
         <v>359</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
         <v>359</v>
-      </c>
-      <c r="F13" s="21" t="s">
-        <v>359</v>
-      </c>
-      <c r="I13" s="11" t="s">
-        <v>359</v>
-      </c>
-      <c r="J13" s="11" t="s">
-        <v>359</v>
-      </c>
-      <c r="K13" t="s">
-        <v>359</v>
-      </c>
-      <c r="N13" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>390</v>
-      </c>
-      <c r="C14" s="53" t="str">
-        <f>HYPERLINK("https://support.twilio.com/hc/en-us/articles/223136027-Auth-Tokens-and-How-to-Change-Them","Twilio auth token")</f>
-        <v>Twilio auth token</v>
       </c>
       <c r="F14" s="21" t="s">
         <v>359</v>
@@ -5320,7 +5348,7 @@
         <v>359</v>
       </c>
       <c r="N14" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="15" spans="1:23" ht="17" x14ac:dyDescent="0.2">
@@ -5328,65 +5356,72 @@
         <v>139</v>
       </c>
       <c r="B15" s="9" t="s">
+        <v>390</v>
+      </c>
+      <c r="C15" s="53" t="str">
+        <f>HYPERLINK("https://support.twilio.com/hc/en-us/articles/223136027-Auth-Tokens-and-How-to-Change-Them","Twilio auth token")</f>
+        <v>Twilio auth token</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>359</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>359</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>359</v>
+      </c>
+      <c r="K15" t="s">
+        <v>359</v>
+      </c>
+      <c r="N15" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B16" s="9" t="s">
         <v>393</v>
       </c>
-      <c r="C15" s="53" t="str">
+      <c r="C16" s="53" t="str">
         <f>HYPERLINK("https://www.twilio.com/docs/phone-numbers","Twilio phone nmber")</f>
         <v>Twilio phone nmber</v>
       </c>
-      <c r="D15" s="21" t="s">
+      <c r="D16" s="21" t="s">
         <v>359</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E16" t="s">
         <v>359</v>
       </c>
-      <c r="F15" s="21" t="s">
+      <c r="F16" s="21" t="s">
         <v>359</v>
       </c>
-      <c r="K15" t="s">
+      <c r="K16" t="s">
         <v>359</v>
       </c>
-      <c r="N15" t="s">
+      <c r="N16" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="16" spans="1:23" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" s="9" t="s">
+    <row r="17" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B17" s="9" t="s">
         <v>376</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C17" s="10" t="s">
         <v>377</v>
       </c>
-      <c r="D16" s="21" t="s">
-        <v>409</v>
-      </c>
-      <c r="E16" t="str">
+      <c r="D17" s="21" t="s">
+        <v>408</v>
+      </c>
+      <c r="E17" t="str">
         <f>"+1"</f>
         <v>+1</v>
       </c>
-      <c r="F16" s="21" t="s">
-        <v>378</v>
-      </c>
-      <c r="K16" t="s">
-        <v>379</v>
-      </c>
-      <c r="N16" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>382</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>383</v>
-      </c>
       <c r="F17" s="21" t="s">
         <v>378</v>
       </c>
@@ -5394,24 +5429,27 @@
         <v>379</v>
       </c>
       <c r="N17" t="s">
-        <v>388</v>
+        <v>359</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>297</v>
-      </c>
-      <c r="B18" t="s">
-        <v>384</v>
-      </c>
-      <c r="C18" s="21" t="s">
-        <v>385</v>
-      </c>
-      <c r="E18" s="72">
-        <v>1</v>
+      <c r="A18" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>382</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>383</v>
+      </c>
+      <c r="F18" s="21" t="s">
+        <v>378</v>
       </c>
       <c r="K18" t="s">
         <v>379</v>
+      </c>
+      <c r="N18" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="17" x14ac:dyDescent="0.2">
@@ -5419,16 +5457,13 @@
         <v>297</v>
       </c>
       <c r="B19" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>387</v>
-      </c>
-      <c r="E19" t="s">
-        <v>361</v>
-      </c>
-      <c r="F19" s="21" t="s">
-        <v>359</v>
+        <v>385</v>
+      </c>
+      <c r="E19" s="61">
+        <v>1</v>
       </c>
       <c r="K19" t="s">
         <v>379</v>
@@ -5436,96 +5471,89 @@
     </row>
     <row r="20" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>154</v>
+        <v>297</v>
       </c>
       <c r="B20" t="s">
-        <v>397</v>
+        <v>386</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>396</v>
+        <v>387</v>
+      </c>
+      <c r="E20" t="s">
+        <v>361</v>
       </c>
       <c r="F20" s="21" t="s">
         <v>359</v>
       </c>
       <c r="K20" t="s">
-        <v>359</v>
-      </c>
-      <c r="N20" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" ht="119" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>87</v>
-      </c>
-      <c r="B21" t="s">
-        <v>380</v>
-      </c>
-      <c r="C21" s="21" t="s">
-        <v>381</v>
-      </c>
-      <c r="F21" s="21" t="s">
-        <v>417</v>
-      </c>
-      <c r="K21" t="s">
-        <v>374</v>
-      </c>
-      <c r="O21" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" ht="34" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21"/>
+      <c r="B21"/>
+      <c r="C21" s="21"/>
+      <c r="E21"/>
+      <c r="F21" s="21"/>
+      <c r="K21"/>
+      <c r="N21" s="54"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" s="58" t="s">
         <v>139</v>
       </c>
-      <c r="B22" t="s">
-        <v>401</v>
-      </c>
-      <c r="C22" s="21" t="s">
-        <v>411</v>
-      </c>
-      <c r="F22" s="21" t="s">
-        <v>359</v>
-      </c>
-      <c r="K22" t="s">
-        <v>359</v>
-      </c>
-      <c r="N22" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+      <c r="B22" s="58" t="s">
+        <v>438</v>
+      </c>
+      <c r="C22" s="21"/>
+      <c r="E22"/>
+      <c r="F22" s="21"/>
+      <c r="K22"/>
+      <c r="N22" s="54" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>139</v>
+        <v>154</v>
       </c>
       <c r="B23" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>416</v>
-      </c>
-      <c r="I23" t="s">
+        <v>395</v>
+      </c>
+      <c r="F23" s="21" t="s">
         <v>359</v>
       </c>
       <c r="K23" t="s">
         <v>359</v>
       </c>
       <c r="N23" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+        <v>359</v>
+      </c>
+      <c r="O23" s="9" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="119" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>139</v>
+        <v>87</v>
       </c>
       <c r="B24" t="s">
-        <v>405</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>412</v>
-      </c>
-      <c r="N24" t="s">
-        <v>406</v>
+        <v>380</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>381</v>
+      </c>
+      <c r="F24" s="21" t="s">
+        <v>415</v>
+      </c>
+      <c r="K24" t="s">
+        <v>374</v>
+      </c>
+      <c r="O24" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="34" x14ac:dyDescent="0.2">
@@ -5533,137 +5561,253 @@
         <v>139</v>
       </c>
       <c r="B25" t="s">
-        <v>407</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>413</v>
+        <v>400</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>410</v>
+      </c>
+      <c r="F25" s="21" t="s">
+        <v>359</v>
+      </c>
+      <c r="K25" t="s">
+        <v>359</v>
       </c>
       <c r="N25" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>420</v>
-      </c>
-      <c r="B26" s="58" t="s">
-        <v>421</v>
-      </c>
-      <c r="C26" s="55" t="s">
-        <v>422</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>423</v>
-      </c>
-      <c r="F26" s="56"/>
-      <c r="K26" s="54"/>
-      <c r="N26"/>
-      <c r="O26" s="54"/>
-    </row>
-    <row r="27" spans="1:15" ht="51" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+      <c r="B26" t="s">
+        <v>402</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>414</v>
+      </c>
+      <c r="I26" t="s">
+        <v>359</v>
+      </c>
+      <c r="K26" t="s">
+        <v>359</v>
+      </c>
+      <c r="N26" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>297</v>
-      </c>
-      <c r="B27" s="58" t="s">
-        <v>414</v>
-      </c>
-      <c r="C27" s="21" t="s">
-        <v>415</v>
-      </c>
-      <c r="F27" s="21" t="s">
-        <v>425</v>
-      </c>
-      <c r="K27" t="s">
-        <v>379</v>
-      </c>
-      <c r="N27" s="54"/>
-      <c r="O27"/>
-    </row>
-    <row r="28" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+      <c r="B27" t="s">
+        <v>404</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>411</v>
+      </c>
+      <c r="N27" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>139</v>
       </c>
-      <c r="B28" s="58" t="s">
+      <c r="B28" t="s">
+        <v>406</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>412</v>
+      </c>
+      <c r="N28" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>297</v>
+      </c>
+      <c r="B29" s="58" t="s">
+        <v>432</v>
+      </c>
+      <c r="C29" s="55" t="s">
+        <v>433</v>
+      </c>
+      <c r="F29" s="56"/>
+      <c r="K29" s="54"/>
+      <c r="N29"/>
+      <c r="O29" s="54"/>
+    </row>
+    <row r="30" spans="1:15" ht="102" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="58" t="s">
+        <v>434</v>
+      </c>
+      <c r="C30" s="55" t="s">
+        <v>435</v>
+      </c>
+      <c r="F30" s="56"/>
+      <c r="I30" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="K30" s="54"/>
+      <c r="N30"/>
+      <c r="O30" s="54"/>
+    </row>
+    <row r="31" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>297</v>
+      </c>
+      <c r="B31" s="58" t="s">
+        <v>444</v>
+      </c>
+      <c r="C31" s="55" t="s">
+        <v>445</v>
+      </c>
+      <c r="F31" s="56"/>
+      <c r="I31" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="K31" s="54"/>
+      <c r="N31"/>
+      <c r="O31" s="54"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>155</v>
+      </c>
+      <c r="B32" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="68" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" t="s">
+        <v>397</v>
+      </c>
+      <c r="C33" s="21" t="s">
+        <v>398</v>
+      </c>
+      <c r="I33" t="s">
+        <v>399</v>
+      </c>
+      <c r="K33" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A34"/>
+      <c r="B34"/>
+      <c r="C34" s="21"/>
+      <c r="F34" s="56"/>
+      <c r="I34"/>
+      <c r="K34"/>
+      <c r="N34" s="54"/>
+      <c r="O34" s="54"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>139</v>
+      </c>
+      <c r="B35" s="58" t="s">
+        <v>441</v>
+      </c>
+      <c r="C35" s="21"/>
+      <c r="F35" s="56"/>
+      <c r="I35"/>
+      <c r="K35"/>
+      <c r="N35" s="54" t="s">
+        <v>443</v>
+      </c>
+      <c r="O35" s="54"/>
+    </row>
+    <row r="36" spans="1:15" ht="51" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>297</v>
+      </c>
+      <c r="B36" s="58" t="s">
+        <v>413</v>
+      </c>
+      <c r="C36" s="21" t="s">
+        <v>436</v>
+      </c>
+      <c r="F36" s="21" t="s">
+        <v>442</v>
+      </c>
+      <c r="I36" s="9" t="s">
+        <v>446</v>
+      </c>
+      <c r="K36" t="s">
+        <v>379</v>
+      </c>
+      <c r="N36" s="54"/>
+      <c r="O36"/>
+    </row>
+    <row r="37" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>139</v>
+      </c>
+      <c r="B37" s="58" t="s">
+        <v>424</v>
+      </c>
+      <c r="C37" s="21" t="s">
         <v>428</v>
       </c>
-      <c r="C28" s="21" t="s">
-        <v>432</v>
-      </c>
-      <c r="F28" s="21"/>
-      <c r="K28"/>
-      <c r="N28" s="71" t="s">
+      <c r="F37" s="21"/>
+      <c r="K37"/>
+      <c r="N37" s="60" t="s">
+        <v>423</v>
+      </c>
+      <c r="O37"/>
+    </row>
+    <row r="38" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>139</v>
+      </c>
+      <c r="B38" s="58" t="s">
+        <v>425</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>429</v>
+      </c>
+      <c r="F38" s="21"/>
+      <c r="K38"/>
+      <c r="N38" s="60" t="s">
         <v>427</v>
       </c>
-      <c r="O28"/>
-    </row>
-    <row r="29" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="O38"/>
+    </row>
+    <row r="39" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>139</v>
       </c>
-      <c r="B29" s="58" t="s">
-        <v>429</v>
-      </c>
-      <c r="C29" s="21" t="s">
-        <v>433</v>
-      </c>
-      <c r="F29" s="21"/>
-      <c r="K29"/>
-      <c r="N29" s="71" t="s">
-        <v>431</v>
-      </c>
-      <c r="O29"/>
-    </row>
-    <row r="30" spans="1:15" ht="34" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>139</v>
-      </c>
-      <c r="B30" s="58" t="s">
+      <c r="B39" s="58" t="s">
+        <v>422</v>
+      </c>
+      <c r="C39" s="21" t="s">
+        <v>430</v>
+      </c>
+      <c r="F39" s="21"/>
+      <c r="K39"/>
+      <c r="N39" s="60" t="s">
         <v>426</v>
       </c>
-      <c r="C30" s="21" t="s">
-        <v>434</v>
-      </c>
-      <c r="F30" s="21"/>
-      <c r="K30"/>
-      <c r="N30" s="71" t="s">
-        <v>430</v>
-      </c>
-      <c r="O30"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>155</v>
-      </c>
-      <c r="B31" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" ht="68" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>33</v>
-      </c>
-      <c r="B32" t="s">
-        <v>398</v>
-      </c>
-      <c r="C32" s="21" t="s">
-        <v>399</v>
-      </c>
-      <c r="I32" t="s">
-        <v>400</v>
-      </c>
-      <c r="K32" t="s">
-        <v>374</v>
-      </c>
+      <c r="O39"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="I1:I1048576 F1:F1048576 B1:C1048576">
+  <conditionalFormatting sqref="F1:F1048576 B1:C1048576 I1:I1048576">
     <cfRule type="expression" dxfId="133" priority="49" stopIfTrue="1">
       <formula>$A1="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O1:O1048576 I1:I1048576 B1:C1048576">
+  <conditionalFormatting sqref="O1:O1048576 B1:C1048576 I1:I1048576">
     <cfRule type="expression" dxfId="132" priority="46" stopIfTrue="1">
       <formula>$A1="begin repeat"</formula>
     </cfRule>
@@ -5858,29 +6002,29 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
+        <v>419</v>
+      </c>
+      <c r="B5" s="15" t="s">
         <v>421</v>
       </c>
-      <c r="B5" s="15" t="s">
-        <v>424</v>
-      </c>
       <c r="C5" s="15" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>24</v>
@@ -5971,14 +6115,14 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2008291916</v>
+        <v>2009012012</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>359</v>
@@ -6013,22 +6157,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="60"/>
+      <c r="B1" s="63"/>
       <c r="C1" s="32"/>
     </row>
     <row r="2" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="61"/>
-      <c r="B2" s="62"/>
+      <c r="A2" s="64"/>
+      <c r="B2" s="65"/>
       <c r="C2" s="32"/>
     </row>
     <row r="3" spans="1:30" s="33" customFormat="1" ht="97" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="66" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="64"/>
+      <c r="B3" s="67"/>
       <c r="C3" s="32"/>
     </row>
     <row r="4" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.2">
@@ -6222,10 +6366,10 @@
       <c r="C7" s="32"/>
     </row>
     <row r="8" spans="1:30" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="65" t="s">
+      <c r="A8" s="68" t="s">
         <v>267</v>
       </c>
-      <c r="B8" s="65"/>
+      <c r="B8" s="68"/>
       <c r="C8" s="40"/>
       <c r="D8" s="41"/>
       <c r="E8" s="41"/>
@@ -6570,7 +6714,7 @@
       <c r="AC17" s="43"/>
       <c r="AD17" s="43"/>
     </row>
-    <row r="18" spans="1:30" s="45" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" s="45" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" s="43" t="s">
         <v>93</v>
       </c>
@@ -9015,10 +9159,10 @@
       <c r="AD81" s="43"/>
     </row>
     <row r="83" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="66" t="s">
+      <c r="A83" s="69" t="s">
         <v>263</v>
       </c>
-      <c r="B83" s="67"/>
+      <c r="B83" s="70"/>
       <c r="C83" s="26"/>
       <c r="D83" s="25"/>
       <c r="E83" s="30"/>
@@ -10178,20 +10322,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="60"/>
+      <c r="B1" s="63"/>
     </row>
     <row r="2" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="61"/>
-      <c r="B2" s="62"/>
+      <c r="A2" s="64"/>
+      <c r="B2" s="65"/>
     </row>
     <row r="3" spans="1:8" s="33" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="64"/>
+      <c r="B3" s="67"/>
     </row>
     <row r="4" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:8" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -10266,28 +10410,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="71" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="69"/>
+      <c r="B1" s="72"/>
       <c r="C1" s="49"/>
       <c r="D1" s="49"/>
       <c r="E1" s="49"/>
       <c r="F1" s="49"/>
     </row>
     <row r="2" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="61"/>
-      <c r="B2" s="62"/>
+      <c r="A2" s="64"/>
+      <c r="B2" s="65"/>
       <c r="C2" s="49"/>
       <c r="D2" s="49"/>
       <c r="E2" s="49"/>
       <c r="F2" s="49"/>
     </row>
     <row r="3" spans="1:8" s="33" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="64"/>
+      <c r="B3" s="67"/>
       <c r="C3" s="49"/>
       <c r="D3" s="49"/>
       <c r="E3" s="49"/>

</xml_diff>

<commit_message>
Made more fields required
</commit_message>
<xml_diff>
--- a/extras/sample-form/Sample form - Delete Twilio recording.xlsx
+++ b/extras/sample-form/Sample form - Delete Twilio recording.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Dobility support/Field plug-ins/Plug-ins by Max/In progress/twilio-control/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E6ADAD-BAF2-134E-B0F4-57DE7C63B0A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE02427-5FAD-E045-AE99-5397A942E5F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28740" yWindow="460" windowWidth="28800" windowHeight="16720" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="460" windowWidth="28800" windowHeight="16720" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="448">
   <si>
     <t>type</t>
   </si>
@@ -5010,7 +5010,7 @@
   <dimension ref="A1:W39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A40" sqref="A40"/>
@@ -5314,7 +5314,9 @@
         <v>420</v>
       </c>
       <c r="F13" s="56"/>
-      <c r="K13" s="54"/>
+      <c r="K13" s="54" t="s">
+        <v>379</v>
+      </c>
       <c r="N13"/>
       <c r="O13" s="54"/>
     </row>
@@ -5635,7 +5637,9 @@
         <v>433</v>
       </c>
       <c r="F29" s="56"/>
-      <c r="K29" s="54"/>
+      <c r="K29" s="54" t="s">
+        <v>379</v>
+      </c>
       <c r="N29"/>
       <c r="O29" s="54"/>
     </row>
@@ -5671,7 +5675,9 @@
       <c r="I31" s="9" t="s">
         <v>437</v>
       </c>
-      <c r="K31" s="54"/>
+      <c r="K31" s="54" t="s">
+        <v>379</v>
+      </c>
       <c r="N31"/>
       <c r="O31" s="54"/>
     </row>
@@ -6122,7 +6128,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2009012012</v>
+        <v>2009112021</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>359</v>
@@ -6714,7 +6720,7 @@
       <c r="AC17" s="43"/>
       <c r="AD17" s="43"/>
     </row>
-    <row r="18" spans="1:30" s="45" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" s="45" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="43" t="s">
         <v>93</v>
       </c>

</xml_diff>

<commit_message>
Made other field required
</commit_message>
<xml_diff>
--- a/extras/sample-form/Sample form - Delete Twilio recording.xlsx
+++ b/extras/sample-form/Sample form - Delete Twilio recording.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Dobility support/Field plug-ins/Plug-ins by Max/In progress/twilio-control/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE02427-5FAD-E045-AE99-5397A942E5F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5A81AB-BCD3-A14D-AD66-5B2B4703E968}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28800" yWindow="460" windowWidth="28800" windowHeight="16720" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5010,7 +5010,7 @@
   <dimension ref="A1:W39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A40" sqref="A40"/>
@@ -5552,7 +5552,7 @@
         <v>415</v>
       </c>
       <c r="K24" t="s">
-        <v>374</v>
+        <v>379</v>
       </c>
       <c r="O24" t="s">
         <v>359</v>
@@ -6128,7 +6128,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2009112021</v>
+        <v>2009112024</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>359</v>

</xml_diff>